<commit_message>
refactored code to remove duplicates
</commit_message>
<xml_diff>
--- a/src/test/resources/customer.xlsx
+++ b/src/test/resources/customer.xlsx
@@ -55,31 +55,31 @@
     <t>customer1</t>
   </si>
   <si>
+    <t>homePhone</t>
+  </si>
+  <si>
+    <t>cellPhone</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>reference:phone@id#1</t>
+  </si>
+  <si>
+    <t>street address2</t>
+  </si>
+  <si>
+    <t>street address1</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
     <t>address</t>
   </si>
   <si>
-    <t>homePhone</t>
-  </si>
-  <si>
-    <t>cellPhone</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>reference:phone@id#1</t>
-  </si>
-  <si>
-    <t>reference:address@id#1</t>
-  </si>
-  <si>
-    <t>street address2</t>
-  </si>
-  <si>
-    <t>street address1</t>
-  </si>
-  <si>
-    <t>New York</t>
+    <t>listReference:address@id#1,address@id#2</t>
   </si>
 </sst>
 </file>
@@ -439,6 +439,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -453,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -467,7 +468,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -480,7 +481,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -515,10 +516,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>12345</v>
@@ -527,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -535,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3">
         <v>54321</v>
@@ -547,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -570,10 +571,10 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>